<commit_message>
Added Hyperlink to Issue title
</commit_message>
<xml_diff>
--- a/static/triton_bugs_dataset.xlsx
+++ b/static/triton_bugs_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/121ecc67766ef65b/01_Academic/Triton Bug/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="11_F25DC773A252ABDACC1048790118673A5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7986F2CC-9263-4DB0-8AD2-5472264A091D}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="11_F25DC773A252ABDACC1048790118673A5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41AFF24F-74E4-4CDE-B55A-7B5F6A706039}"/>
   <bookViews>
-    <workbookView xWindow="16371" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>Hang</t>
   </si>
   <si>
-    <t>xformers</t>
-  </si>
-  <si>
     <t>Blocksparse forced to use FP16 when BF16 is supported (for triton v2) #353</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>[Bug]: Triton error when initializing LLM(...) when enable_lora=True and cuda device != cuda:0 #12967</t>
   </si>
   <si>
-    <t>Intel</t>
-  </si>
-  <si>
     <t>Triton FP8 data type support #322</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>[PyTorch Upstream] Triton crash when compile torch.nn.functional.interpolate.bicubic #829</t>
   </si>
   <si>
-    <t>Trtiton</t>
-  </si>
-  <si>
     <t>Bug of TRITON_OVERRIDE #6113</t>
   </si>
   <si>
@@ -330,9 +321,6 @@
     <t>[Interpreter] The Triton interpreter doesn't support the int1 type. #6200</t>
   </si>
   <si>
-    <t>flag gem</t>
-  </si>
-  <si>
     <t>Reduction Op Softmax, Cross Entropy Loss, and LogSoftmax Test Failed While Parsing JITFunc in Triton #110</t>
   </si>
   <si>
@@ -457,6 +445,18 @@
   </si>
   <si>
     <t>Different Libraries</t>
+  </si>
+  <si>
+    <t>facebookresearch/xformers</t>
+  </si>
+  <si>
+    <t>intel/intel-xpu-backend-for-triton</t>
+  </si>
+  <si>
+    <t>triton-lang/triton</t>
+  </si>
+  <si>
+    <t>FlagOpen/FlagGems</t>
   </si>
 </sst>
 </file>
@@ -986,11 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.4609375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1003,7 +1002,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1012,22 +1011,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1038,22 +1037,22 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1064,22 +1063,22 @@
         <v>4</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1090,22 +1089,22 @@
         <v>5</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1116,22 +1115,22 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1142,19 +1141,19 @@
         <v>8</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.4">
@@ -1168,22 +1167,22 @@
         <v>9</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1194,22 +1193,22 @@
         <v>10</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1220,1465 +1219,1453 @@
         <v>10</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="B10" s="8">
         <v>353</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="B11" s="12">
         <v>206</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="H11" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="B12" s="12">
         <v>519</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="B13" s="5">
         <v>12967</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B14" s="8">
         <v>322</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B15" s="12">
         <v>787</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="10" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B16" s="15">
         <v>3704</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="10" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B17" s="15">
         <v>3641</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="10" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B18" s="15">
         <v>3090</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="10" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B19" s="15">
         <v>3072</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B20" s="15">
         <v>1126</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B21" s="15">
         <v>1125</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="10" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B22" s="15">
         <v>881</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B23" s="15">
         <v>829</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B24" s="8">
         <v>6113</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B25" s="15">
         <v>6034</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B26" s="15">
         <v>5882</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B27" s="15">
         <v>5791</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B28" s="15">
         <v>5745</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B29" s="15">
         <v>5620</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B30" s="15">
         <v>5494</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B31" s="15">
         <v>5491</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B32" s="15">
         <v>1047</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B33" s="15">
         <v>989</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B34" s="15">
         <v>4492</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B35" s="15">
         <v>4418</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B36" s="15">
         <v>4317</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B37" s="15">
         <v>3467</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B38" s="15">
         <v>2662</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B39" s="15">
         <v>3310</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B40" s="15">
         <v>3013</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E40" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="G40" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B41" s="15">
         <v>2821</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B42" s="15">
         <v>2523</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B43" s="15">
         <v>2361</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B44" s="15">
         <v>2298</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B45" s="15">
         <v>2231</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B46" s="15">
         <v>1864</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B47" s="15">
         <v>1846</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B48" s="15">
         <v>1715</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B49" s="15">
         <v>1670</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B50" s="15">
         <v>1621</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B51" s="15">
         <v>1330</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B52" s="12">
         <v>1162</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B53" s="15">
         <v>6958</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B54" s="15">
         <v>6748</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B55" s="15">
         <v>6547</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B56" s="15">
         <v>6346</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F56" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G56" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="G56" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="H56" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B57" s="15">
         <v>6292</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B58" s="15">
         <v>6251</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B59" s="15">
         <v>6220</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B60" s="15">
         <v>6219</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="10" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B61" s="15">
         <v>6200</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="19" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="B62" s="20">
         <v>110</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="19" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="B63" s="15">
         <v>124</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="19" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="B64" s="12">
         <v>267</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H64" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Wrong Result"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters>
-        <filter val="different libraries"/>
-        <filter val="library differences"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{88694323-157A-47FC-9C6B-A1DB00B1E9AB}"/>
     <hyperlink ref="C13" r:id="rId2" display="[Bug]: Triton error when initializing `LLM(...)` when `enable_lora=True` and `cuda` device != `cuda:0` · Issue #12967 · vllm-project/vllm · GitHub" xr:uid="{BF5FF7C2-8319-4E8B-B846-CA27902B86A6}"/>

</xml_diff>